<commit_message>
Add pin-canonicals parameter to sushi-config.yaml 21e610ea36eba4d6068763059a8724ca779a524f
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-EyeColor.xlsx
+++ b/main/ig/StructureDefinition-EyeColor.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-03T08:52:56+00:00</t>
+    <t>2025-12-19T08:24:59+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -108,7 +108,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/StructureDefinition/Extension</t>
+    <t>http://hl7.org/fhir/StructureDefinition/Extension|4.0.1</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -341,7 +341,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/[code]/ValueSet/EyeColorVS</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/[code]/ValueSet/EyeColorVS|0.1.0</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
@@ -690,7 +690,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="51.87890625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="56.41015625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>

</xml_diff>